<commit_message>
Urban Ladder price is modified
</commit_message>
<xml_diff>
--- a/BookShelves.xlsx
+++ b/BookShelves.xlsx
@@ -12,13 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Theodore Open Display Cabinet</t>
-  </si>
-  <si>
-    <t>₹12,239</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Rhodes Folding Book Shelf</t>
   </si>
@@ -30,6 +24,9 @@
   </si>
   <si>
     <t>₹8,249</t>
+  </si>
+  <si>
+    <t>₹12,039</t>
   </si>
 </sst>
 </file>
@@ -80,7 +77,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="29.35546875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="28.203125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -101,10 +98,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>